<commit_message>
added results and enhanced matlab script
</commit_message>
<xml_diff>
--- a/pyFiles/MPC/Results/ResultsMPC.xlsx
+++ b/pyFiles/MPC/Results/ResultsMPC.xlsx
@@ -5,12 +5,12 @@
   <workbookPr defaultThemeVersion="166925"/>
   <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
     <mc:Choice Requires="x15">
-      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\axkar1\Documents\GitProj\ThesisWorkCybercom-master\pyFiles\MPC\Results\"/>
+      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\axkar1\Documents\MATLAB\pyFiles\MPC\Results\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{42DEB79C-8F04-497E-BA1D-E71F9AC45410}" xr6:coauthVersionLast="41" xr6:coauthVersionMax="41" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{4F0B8237-CDD4-4BE1-BEE1-1E22E8C752D8}" xr6:coauthVersionLast="41" xr6:coauthVersionMax="41" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="3660" yWindow="1308" windowWidth="17280" windowHeight="8964" xr2:uid="{1BC5E51A-5632-4252-887C-9C128D35FB87}"/>
+    <workbookView xWindow="4245" yWindow="4245" windowWidth="28800" windowHeight="15435" xr2:uid="{1BC5E51A-5632-4252-887C-9C128D35FB87}"/>
   </bookViews>
   <sheets>
     <sheet name="Sheet1" sheetId="1" r:id="rId1"/>
@@ -31,7 +31,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="27" uniqueCount="16">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="39" uniqueCount="20">
   <si>
     <t>Controller</t>
   </si>
@@ -79,6 +79,18 @@
   </si>
   <si>
     <t>Horizon Length [segm]</t>
+  </si>
+  <si>
+    <t>3, 223, 568</t>
+  </si>
+  <si>
+    <t>3, 114, 741</t>
+  </si>
+  <si>
+    <t>688, 089</t>
+  </si>
+  <si>
+    <t>711, 428</t>
   </si>
 </sst>
 </file>
@@ -110,7 +122,6 @@
     </font>
     <font>
       <sz val="11"/>
-      <color rgb="FFFF0000"/>
       <name val="Calibri"/>
       <family val="2"/>
       <scheme val="minor"/>
@@ -474,20 +485,20 @@
   <dimension ref="A1:F45"/>
   <sheetViews>
     <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="E12" sqref="E12"/>
+      <selection activeCell="F17" sqref="F17"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr defaultRowHeight="14.4" x14ac:dyDescent="0.3"/>
+  <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
   <cols>
-    <col min="1" max="1" width="13.109375" customWidth="1"/>
-    <col min="2" max="2" width="33.44140625" customWidth="1"/>
-    <col min="3" max="3" width="14.33203125" customWidth="1"/>
-    <col min="4" max="4" width="26.5546875" customWidth="1"/>
-    <col min="5" max="5" width="18.33203125" customWidth="1"/>
-    <col min="6" max="6" width="13.33203125" customWidth="1"/>
+    <col min="1" max="1" width="13.140625" customWidth="1"/>
+    <col min="2" max="2" width="33.42578125" customWidth="1"/>
+    <col min="3" max="3" width="14.28515625" customWidth="1"/>
+    <col min="4" max="4" width="26.5703125" customWidth="1"/>
+    <col min="5" max="5" width="18.28515625" customWidth="1"/>
+    <col min="6" max="6" width="13.28515625" customWidth="1"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:6" ht="30.75" customHeight="1" x14ac:dyDescent="0.35">
+    <row r="1" spans="1:6" ht="30.75" customHeight="1" x14ac:dyDescent="0.3">
       <c r="A1" s="2" t="s">
         <v>0</v>
       </c>
@@ -507,7 +518,7 @@
         <v>6</v>
       </c>
     </row>
-    <row r="2" spans="1:6" x14ac:dyDescent="0.3">
+    <row r="2" spans="1:6" x14ac:dyDescent="0.25">
       <c r="A2" s="3" t="s">
         <v>1</v>
       </c>
@@ -527,7 +538,7 @@
         <v>7</v>
       </c>
     </row>
-    <row r="3" spans="1:6" x14ac:dyDescent="0.3">
+    <row r="3" spans="1:6" x14ac:dyDescent="0.25">
       <c r="A3" s="4"/>
       <c r="B3" s="1" t="s">
         <v>11</v>
@@ -545,8 +556,10 @@
         <v>7</v>
       </c>
     </row>
-    <row r="4" spans="1:6" x14ac:dyDescent="0.3">
-      <c r="A4" s="4"/>
+    <row r="4" spans="1:6" x14ac:dyDescent="0.25">
+      <c r="A4" s="4">
+        <v>1</v>
+      </c>
       <c r="B4" s="1" t="s">
         <v>13</v>
       </c>
@@ -563,8 +576,10 @@
         <v>7</v>
       </c>
     </row>
-    <row r="5" spans="1:6" x14ac:dyDescent="0.3">
-      <c r="A5" s="4"/>
+    <row r="5" spans="1:6" x14ac:dyDescent="0.25">
+      <c r="A5" s="4">
+        <v>2</v>
+      </c>
       <c r="B5" s="1" t="s">
         <v>8</v>
       </c>
@@ -581,9 +596,19 @@
         <v>7</v>
       </c>
     </row>
-    <row r="6" spans="1:6" x14ac:dyDescent="0.3">
-      <c r="A6" s="4"/>
-      <c r="B6" s="1"/>
+    <row r="6" spans="1:6" x14ac:dyDescent="0.25">
+      <c r="A6" s="4">
+        <v>3</v>
+      </c>
+      <c r="B6" s="1" t="s">
+        <v>16</v>
+      </c>
+      <c r="C6">
+        <v>999</v>
+      </c>
+      <c r="D6">
+        <v>10</v>
+      </c>
       <c r="E6">
         <v>1</v>
       </c>
@@ -591,9 +616,19 @@
         <v>7</v>
       </c>
     </row>
-    <row r="7" spans="1:6" x14ac:dyDescent="0.3">
-      <c r="A7" s="4"/>
-      <c r="B7" s="1"/>
+    <row r="7" spans="1:6" x14ac:dyDescent="0.25">
+      <c r="A7" s="4">
+        <v>4</v>
+      </c>
+      <c r="B7" s="1" t="s">
+        <v>17</v>
+      </c>
+      <c r="C7">
+        <v>919</v>
+      </c>
+      <c r="D7">
+        <v>10</v>
+      </c>
       <c r="E7">
         <v>1</v>
       </c>
@@ -601,8 +636,10 @@
         <v>7</v>
       </c>
     </row>
-    <row r="8" spans="1:6" x14ac:dyDescent="0.3">
-      <c r="A8" s="4"/>
+    <row r="8" spans="1:6" x14ac:dyDescent="0.25">
+      <c r="A8" s="4">
+        <v>5</v>
+      </c>
       <c r="B8" s="1"/>
       <c r="E8">
         <v>1</v>
@@ -611,8 +648,10 @@
         <v>7</v>
       </c>
     </row>
-    <row r="9" spans="1:6" x14ac:dyDescent="0.3">
-      <c r="A9" s="4"/>
+    <row r="9" spans="1:6" x14ac:dyDescent="0.25">
+      <c r="A9" s="4">
+        <v>6</v>
+      </c>
       <c r="B9" s="1"/>
       <c r="E9">
         <v>1</v>
@@ -621,8 +660,10 @@
         <v>7</v>
       </c>
     </row>
-    <row r="10" spans="1:6" x14ac:dyDescent="0.3">
-      <c r="A10" s="4"/>
+    <row r="10" spans="1:6" x14ac:dyDescent="0.25">
+      <c r="A10" s="4">
+        <v>7</v>
+      </c>
       <c r="B10" s="1"/>
       <c r="E10">
         <v>1</v>
@@ -631,167 +672,244 @@
         <v>7</v>
       </c>
     </row>
-    <row r="11" spans="1:6" x14ac:dyDescent="0.3">
-      <c r="A11" s="5"/>
+    <row r="11" spans="1:6" x14ac:dyDescent="0.25">
+      <c r="A11" s="5">
+        <v>8</v>
+      </c>
       <c r="B11" s="6"/>
       <c r="C11" s="7"/>
       <c r="D11" s="7"/>
       <c r="E11" s="7"/>
       <c r="F11" s="6"/>
     </row>
-    <row r="12" spans="1:6" x14ac:dyDescent="0.3">
-      <c r="A12" s="3" t="s">
-        <v>2</v>
-      </c>
-      <c r="B12" s="1" t="s">
-        <v>14</v>
-      </c>
-      <c r="C12">
-        <v>15468</v>
-      </c>
-      <c r="E12">
-        <v>1</v>
-      </c>
-      <c r="F12" s="1" t="s">
-        <v>7</v>
-      </c>
-    </row>
-    <row r="13" spans="1:6" x14ac:dyDescent="0.3">
-      <c r="A13" s="4"/>
-      <c r="B13" s="1" t="s">
+    <row r="12" spans="1:6" x14ac:dyDescent="0.25">
+      <c r="A12" s="4">
         <v>9</v>
       </c>
-      <c r="C13">
-        <v>12641</v>
-      </c>
-      <c r="E13">
-        <v>1</v>
-      </c>
-      <c r="F13" s="1" t="s">
-        <v>7</v>
-      </c>
-    </row>
-    <row r="14" spans="1:6" x14ac:dyDescent="0.3">
-      <c r="A14" s="4"/>
-      <c r="B14" s="1"/>
-      <c r="E14">
-        <v>1</v>
-      </c>
-      <c r="F14" s="1" t="s">
-        <v>7</v>
-      </c>
-    </row>
-    <row r="15" spans="1:6" x14ac:dyDescent="0.3">
+    </row>
+    <row r="13" spans="1:6" x14ac:dyDescent="0.25">
+      <c r="A13" s="4">
+        <v>10</v>
+      </c>
+    </row>
+    <row r="15" spans="1:6" x14ac:dyDescent="0.25">
       <c r="A15" s="4"/>
       <c r="B15" s="1"/>
     </row>
-    <row r="16" spans="1:6" x14ac:dyDescent="0.3">
-      <c r="A16" s="4"/>
-      <c r="B16" s="1"/>
-    </row>
-    <row r="17" spans="1:2" x14ac:dyDescent="0.3">
-      <c r="A17" s="4"/>
-      <c r="B17" s="1"/>
-    </row>
-    <row r="18" spans="1:2" x14ac:dyDescent="0.3">
-      <c r="A18" s="4"/>
-      <c r="B18" s="1"/>
-    </row>
-    <row r="19" spans="1:2" x14ac:dyDescent="0.3">
-      <c r="A19" s="4"/>
-      <c r="B19" s="1"/>
-    </row>
-    <row r="20" spans="1:2" x14ac:dyDescent="0.3">
-      <c r="A20" s="4"/>
-      <c r="B20" s="1"/>
-    </row>
-    <row r="21" spans="1:2" x14ac:dyDescent="0.3">
-      <c r="A21" s="4"/>
+    <row r="16" spans="1:6" x14ac:dyDescent="0.25">
+      <c r="A16" s="3" t="s">
+        <v>2</v>
+      </c>
+    </row>
+    <row r="17" spans="1:6" x14ac:dyDescent="0.25">
+      <c r="A17" s="4">
+        <v>1</v>
+      </c>
+      <c r="B17" s="1" t="s">
+        <v>14</v>
+      </c>
+      <c r="C17">
+        <v>15468</v>
+      </c>
+      <c r="E17">
+        <v>1</v>
+      </c>
+      <c r="F17" s="1" t="s">
+        <v>7</v>
+      </c>
+    </row>
+    <row r="18" spans="1:6" x14ac:dyDescent="0.25">
+      <c r="A18" s="4">
+        <v>2</v>
+      </c>
+      <c r="B18" s="1" t="s">
+        <v>9</v>
+      </c>
+      <c r="C18">
+        <v>12641</v>
+      </c>
+      <c r="E18">
+        <v>1</v>
+      </c>
+      <c r="F18" s="1" t="s">
+        <v>7</v>
+      </c>
+    </row>
+    <row r="19" spans="1:6" x14ac:dyDescent="0.25">
+      <c r="A19" s="4">
+        <v>3</v>
+      </c>
+      <c r="B19" s="1" t="s">
+        <v>19</v>
+      </c>
+      <c r="C19">
+        <v>11829</v>
+      </c>
+      <c r="E19">
+        <v>1</v>
+      </c>
+      <c r="F19" s="1" t="s">
+        <v>7</v>
+      </c>
+    </row>
+    <row r="20" spans="1:6" x14ac:dyDescent="0.25">
+      <c r="A20" s="4">
+        <v>4</v>
+      </c>
+      <c r="B20" s="1" t="s">
+        <v>18</v>
+      </c>
+      <c r="C20">
+        <v>12516</v>
+      </c>
+      <c r="E20">
+        <v>1</v>
+      </c>
+      <c r="F20" s="1" t="s">
+        <v>7</v>
+      </c>
+    </row>
+    <row r="21" spans="1:6" x14ac:dyDescent="0.25">
+      <c r="A21" s="4">
+        <v>5</v>
+      </c>
       <c r="B21" s="1"/>
-    </row>
-    <row r="22" spans="1:2" x14ac:dyDescent="0.3">
-      <c r="A22" s="4"/>
+      <c r="E21">
+        <v>1</v>
+      </c>
+      <c r="F21" s="1" t="s">
+        <v>7</v>
+      </c>
+    </row>
+    <row r="22" spans="1:6" x14ac:dyDescent="0.25">
+      <c r="A22" s="4">
+        <v>6</v>
+      </c>
       <c r="B22" s="1"/>
-    </row>
-    <row r="23" spans="1:2" x14ac:dyDescent="0.3">
-      <c r="A23" s="4"/>
+      <c r="E22">
+        <v>1</v>
+      </c>
+      <c r="F22" s="1" t="s">
+        <v>7</v>
+      </c>
+    </row>
+    <row r="23" spans="1:6" x14ac:dyDescent="0.25">
+      <c r="A23" s="4">
+        <v>7</v>
+      </c>
       <c r="B23" s="1"/>
-    </row>
-    <row r="24" spans="1:2" x14ac:dyDescent="0.3">
-      <c r="A24" s="4"/>
+      <c r="E23">
+        <v>1</v>
+      </c>
+      <c r="F23" s="1" t="s">
+        <v>7</v>
+      </c>
+    </row>
+    <row r="24" spans="1:6" x14ac:dyDescent="0.25">
+      <c r="A24" s="4">
+        <v>8</v>
+      </c>
       <c r="B24" s="1"/>
-    </row>
-    <row r="25" spans="1:2" x14ac:dyDescent="0.3">
-      <c r="A25" s="4"/>
+      <c r="E24">
+        <v>1</v>
+      </c>
+      <c r="F24" s="1" t="s">
+        <v>7</v>
+      </c>
+    </row>
+    <row r="25" spans="1:6" x14ac:dyDescent="0.25">
+      <c r="A25" s="4">
+        <v>9</v>
+      </c>
       <c r="B25" s="1"/>
-    </row>
-    <row r="26" spans="1:2" x14ac:dyDescent="0.3">
-      <c r="A26" s="4"/>
+      <c r="E25">
+        <v>1</v>
+      </c>
+      <c r="F25" s="1" t="s">
+        <v>7</v>
+      </c>
+    </row>
+    <row r="26" spans="1:6" x14ac:dyDescent="0.25">
+      <c r="A26" s="4">
+        <v>10</v>
+      </c>
       <c r="B26" s="1"/>
-    </row>
-    <row r="27" spans="1:2" x14ac:dyDescent="0.3">
+      <c r="E26">
+        <v>1</v>
+      </c>
+      <c r="F26" s="1" t="s">
+        <v>7</v>
+      </c>
+    </row>
+    <row r="27" spans="1:6" x14ac:dyDescent="0.25">
       <c r="A27" s="4"/>
       <c r="B27" s="1"/>
-    </row>
-    <row r="28" spans="1:2" x14ac:dyDescent="0.3">
+      <c r="E27">
+        <v>1</v>
+      </c>
+      <c r="F27" s="1" t="s">
+        <v>7</v>
+      </c>
+    </row>
+    <row r="28" spans="1:6" x14ac:dyDescent="0.25">
       <c r="A28" s="4"/>
       <c r="B28" s="1"/>
     </row>
-    <row r="29" spans="1:2" x14ac:dyDescent="0.3">
+    <row r="29" spans="1:6" x14ac:dyDescent="0.25">
       <c r="A29" s="4"/>
       <c r="B29" s="1"/>
     </row>
-    <row r="30" spans="1:2" x14ac:dyDescent="0.3">
+    <row r="30" spans="1:6" x14ac:dyDescent="0.25">
       <c r="A30" s="4"/>
       <c r="B30" s="1"/>
     </row>
-    <row r="31" spans="1:2" x14ac:dyDescent="0.3">
+    <row r="31" spans="1:6" x14ac:dyDescent="0.25">
       <c r="A31" s="4"/>
       <c r="B31" s="1"/>
     </row>
-    <row r="32" spans="1:2" x14ac:dyDescent="0.3">
+    <row r="32" spans="1:6" x14ac:dyDescent="0.25">
       <c r="A32" s="4"/>
       <c r="B32" s="1"/>
     </row>
-    <row r="33" spans="1:2" x14ac:dyDescent="0.3">
+    <row r="33" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A33" s="4"/>
       <c r="B33" s="1"/>
     </row>
-    <row r="34" spans="1:2" x14ac:dyDescent="0.3">
+    <row r="34" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A34" s="4"/>
       <c r="B34" s="1"/>
     </row>
-    <row r="35" spans="1:2" x14ac:dyDescent="0.3">
+    <row r="35" spans="1:2" x14ac:dyDescent="0.25">
       <c r="B35" s="1"/>
     </row>
-    <row r="36" spans="1:2" x14ac:dyDescent="0.3">
+    <row r="36" spans="1:2" x14ac:dyDescent="0.25">
       <c r="B36" s="1"/>
     </row>
-    <row r="37" spans="1:2" x14ac:dyDescent="0.3">
+    <row r="37" spans="1:2" x14ac:dyDescent="0.25">
       <c r="B37" s="1"/>
     </row>
-    <row r="38" spans="1:2" x14ac:dyDescent="0.3">
+    <row r="38" spans="1:2" x14ac:dyDescent="0.25">
       <c r="B38" s="1"/>
     </row>
-    <row r="39" spans="1:2" x14ac:dyDescent="0.3">
+    <row r="39" spans="1:2" x14ac:dyDescent="0.25">
       <c r="B39" s="1"/>
     </row>
-    <row r="40" spans="1:2" x14ac:dyDescent="0.3">
+    <row r="40" spans="1:2" x14ac:dyDescent="0.25">
       <c r="B40" s="1"/>
     </row>
-    <row r="41" spans="1:2" x14ac:dyDescent="0.3">
+    <row r="41" spans="1:2" x14ac:dyDescent="0.25">
       <c r="B41" s="1"/>
     </row>
-    <row r="42" spans="1:2" x14ac:dyDescent="0.3">
+    <row r="42" spans="1:2" x14ac:dyDescent="0.25">
       <c r="B42" s="1"/>
     </row>
-    <row r="43" spans="1:2" x14ac:dyDescent="0.3">
+    <row r="43" spans="1:2" x14ac:dyDescent="0.25">
       <c r="B43" s="1"/>
     </row>
-    <row r="44" spans="1:2" x14ac:dyDescent="0.3">
+    <row r="44" spans="1:2" x14ac:dyDescent="0.25">
       <c r="B44" s="1"/>
     </row>
-    <row r="45" spans="1:2" x14ac:dyDescent="0.3">
+    <row r="45" spans="1:2" x14ac:dyDescent="0.25">
       <c r="B45" s="1"/>
     </row>
   </sheetData>

</xml_diff>